<commit_message>
Added total to FAIR sheet
</commit_message>
<xml_diff>
--- a/FAIR.xlsx
+++ b/FAIR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VIG\work\DMH-Interactive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C730329-F406-4E43-81AF-94D9B31F8E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1DF65C-0B20-4991-8DDF-1D0E0677F19E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1F23D609-0F9E-4EDE-B38D-7135182795E1}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="323">
   <si>
     <t>Score</t>
   </si>
@@ -1101,6 +1101,9 @@
     <t>Data engineer ensures that data are collected and correctly uploaded to NIVA's data storages   
      -   Reporting of data to [Vannmiljø](https://vannmiljo.miljodirektoratet.no)
      -   Quality Assurance</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1522,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19293E65-4AF6-4E51-A593-DC4A92B4B63D}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1535,7 +1538,7 @@
     <col min="3" max="3" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1548,8 +1551,11 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1573,7 +1579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -1597,7 +1603,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1621,7 +1627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1637,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1645,7 +1651,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1661,7 +1667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>